<commit_message>
another problems resolved, new features
</commit_message>
<xml_diff>
--- a/gumshoes.xlsx
+++ b/gumshoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,12 @@
           <t>Image</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr"/>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,6 +460,11 @@
           <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7ba/296_296_2/7baaf1c389ac74050ec7a0c802b39bec.jpg </t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-winter-hi-172348/</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -472,6 +482,11 @@
           <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7fa/296_296_2/7fadf0fd1bcb0f9635cab145ae4cec40.jpg </t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A01330/</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -489,11 +504,16 @@
           <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/196/296_296_2/on8f5v0t97na2ses6mlqpfpkm7ba6is1.jpg </t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-A02771/</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 OX</t>
+          <t>Кеды Converse x Naturally Digital Chuck 70 OX</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -503,524 +523,679 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/585/296_296_2/o25p5xnu007xan8xf118i4tyg8xzqqa0.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/74a/296_296_2/0zprnekw2ewy5x9nobcnbxze9mlwzbr3.jpg </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-A04335/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Кеды Converse x Naturally Digital Chuck 70 OX</t>
+          <t>Кеды Converse Chuck 70 Plus Hi</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>13.500.₽</t>
+          <t>16.000.₽</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/74a/296_296_2/0zprnekw2ewy5x9nobcnbxze9mlwzbr3.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b09/296_296_2/rro1ooz0q455eplhjugznzgzjti9cwbx.jpg </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-plus-hi-A02871/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Кеды Converse x Naturally Digital Chuck 70 Hi</t>
+          <t>Кеды Converse Run Star Motion CX HI</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14.200.₽</t>
+          <t>18.900.₽</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ab5/296_296_2/z4h36lr1v8c3081j1728c42ewh1pv3nr.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f4e/296_296_2/56231v21p308mqunndoa6a6ay31tepzk.jpg </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/run-star-motion-cx-hi-A05110/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 Plus Hi</t>
+          <t>Кеды Converse Run Star Motion CX HI</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16.000.₽</t>
+          <t>19.900.₽</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b09/296_296_2/rro1ooz0q455eplhjugznzgzjti9cwbx.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/59a/296_296_2/btqj3q49w2a4vtsk5txu8u92mhki1qmo.jpg </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/run-star-motion-cx-hi-A04334/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Кеды Converse Run Star Motion CX HI</t>
+          <t>Кеды Converse One Star Pro OX</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18.900.₽</t>
+          <t>13.900.₽</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f4e/296_296_2/56231v21p308mqunndoa6a6ay31tepzk.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/755/296_296_2/h70a0dqk6og8ncmuc559scitlisy3bg4.jpg </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/one-star-pro-ox-A04242/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Кеды Converse Run Star Motion CX HI</t>
+          <t>Кеды Converse Chuck 70 AT-CX Hi</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19.900.₽</t>
+          <t>15.500.₽</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/59a/296_296_2/btqj3q49w2a4vtsk5txu8u92mhki1qmo.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aa7/296_296_2/aq3ojiv2ydjahpzlf1qvbfvbtcxqldhq.jpg </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-at-cx-hi-A02776/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Кеды Converse One Star Pro OX</t>
+          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>13.900.₽</t>
+          <t>17.900.₽</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/755/296_296_2/h70a0dqk6og8ncmuc559scitlisy3bg4.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/924/296_296_2/9247324f208d8ea6585ef112726fd8cf.jpg </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A01765/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 AT-CX Hi</t>
+          <t>Кеды Converse Run Star Hike Hi</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>15.500.₽</t>
+          <t>17.800.₽</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aa7/296_296_2/aq3ojiv2ydjahpzlf1qvbfvbtcxqldhq.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7a1/296_296_2/7a1944071666efd11a4c0aed92011ab6.jpg </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/run-star-hike-hi-A01650/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
+          <t>Кеды Converse Weapon CX Mid</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17.900.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/924/296_296_2/9247324f208d8ea6585ef112726fd8cf.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e6c/296_296_2/e6c0637cb708f993f9afba97bf03a7bb.jpg </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/weapon-cx-mid-A03230/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Кеды Converse Run Star Hike Hi</t>
+          <t>Кеды Converse x CLOT Jack Purcell OX</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17.800.₽</t>
+          <t>16.000.₽</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7a1/296_296_2/7a1944071666efd11a4c0aed92011ab6.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e10/296_296_2/e102471599195bdf15459dfb523ba3bb.jpg </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/jack-purcell-ox-A00322/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Кеды Converse Weapon CX Mid</t>
+          <t>Кеды Converse x CLOT Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>17.200.₽</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e6c/296_296_2/e6c0637cb708f993f9afba97bf03a7bb.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9ec/296_296_2/9ec888598a86778150bc01c8b4ce948e.jpg </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A00321/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Кеды Converse x CLOT Jack Purcell OX</t>
+          <t>Кеды Converse x Come Tees Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16.000.₽</t>
+          <t>17.100.₽</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e10/296_296_2/e102471599195bdf15459dfb523ba3bb.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/05d/296_296_2/05dc34874b3fc00765a1ace5f2c703ae.jpg </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A01762/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Кеды Converse x CLOT Chuck 70 Hi</t>
+          <t>Кеды Converse Chuck 70 Plus Hi</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17.200.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9ec/296_296_2/9ec888598a86778150bc01c8b4ce948e.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a0c/296_296_2/a0c79f03ba520eb75a4ea630fc6d6d07.jpg </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-plus-hi-A00866/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Кеды Converse x Come Tees Chuck 70 Hi</t>
+          <t>Кеды Vans Classic Slip-On 98 DX</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>17.100.₽</t>
+          <t>7.290.₽</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/05d/296_296_2/05dc34874b3fc00765a1ace5f2c703ae.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/25a/296_296_2/25a095a37f2927fe49772808bb99aee4.jpg </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/classic-slip-on-99-DX-VA3JEXPU1/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 Plus Hi</t>
+          <t>Кеды Converse x Carhartt Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>11.900.₽</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a0c/296_296_2/a0c79f03ba520eb75a4ea630fc6d6d07.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/21c/296_296_2/21cc62f5696f9784250ae1f2ffbcc324.jpg </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-carhartt-chuck-70-hi-171237/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Кеды Vans Classic Slip-On 98 DX</t>
+          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7.290.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/25a/296_296_2/25a095a37f2927fe49772808bb99aee4.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aef/296_296_2/aefc82a9c733ffc85cdfec5a013841f5.jpg </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A01329/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Кеды Converse x Carhartt Chuck 70 Hi</t>
+          <t>Кеды Converse x Golf Le Fleur GLF 2.0 OX</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11.900.₽</t>
+          <t>14.500.₽</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/21c/296_296_2/21cc62f5696f9784250ae1f2ffbcc324.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dee/296_296_2/dee01e54df7f8ac297ab6bd21d052bcf.jpg </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-golf-le-fleur-glf-2-0-ox-173186/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
+          <t xml:space="preserve">Кеды Converse x Peanuts One Star OX </t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>16.300.₽</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aef/296_296_2/aefc82a9c733ffc85cdfec5a013841f5.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/558/296_296_2/558930bbdafb92eb1477086be36a9f25.jpg </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/one-star-ox-x-peanuts-A01873/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Кеды Converse x Golf Le Fleur GLF 2.0 OX</t>
+          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>14.500.₽</t>
+          <t>15.300.₽</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dee/296_296_2/dee01e54df7f8ac297ab6bd21d052bcf.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/990/296_296_2/990d5a6329394486464fcd7680e09da6.jpg </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/skid-grip-ox-x-john-elliott-172577/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кеды Converse x Peanuts One Star OX </t>
+          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16.300.₽</t>
+          <t>15.300.₽</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/558/296_296_2/558930bbdafb92eb1477086be36a9f25.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f8/296_296_2/7f89ac7135e6d3c969fdcca189ae6ab8.jpg </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/skid-grip-ox-x-john-elliott-172578/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
+          <t>Кеды Converse x Joshua Vides Weapon CX Hi</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>15.300.₽</t>
+          <t>19.300.₽</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/990/296_296_2/990d5a6329394486464fcd7680e09da6.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bd3/296_296_2/bd3ba0a707a4fe8002fa94c1e2742d99.jpg </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-joshua-vides-weapon-cx-hi-A00715/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
+          <t>Кеды Converse x Carhartt Fastbreak Pro Mid</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>15.300.₽</t>
+          <t>11.100.₽</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f8/296_296_2/7f89ac7135e6d3c969fdcca189ae6ab8.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8de/296_296_2/8de985a56482f5b6c49dd439297fba5c.jpg </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-carhartt-fastbreak-pro-mid-172583/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Кеды Converse x Joshua Vides Weapon CX Hi</t>
+          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>19.300.₽</t>
+          <t>16.300.₽</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bd3/296_296_2/bd3ba0a707a4fe8002fa94c1e2742d99.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fdc/296_296_2/fdcab0e4271fc593d0dc2dbca4b630b4.jpg </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A02052/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Кеды Converse x Carhartt Fastbreak Pro Mid</t>
+          <t>Кеды Converse Chuck 70 OX x GOLF WANG</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11.100.₽</t>
+          <t>13.200.₽</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8de/296_296_2/8de985a56482f5b6c49dd439297fba5c.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e08/296_296_2/e08a58dd412f316675832c861c941994.jpg </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-wang-A01798/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
+          <t>Кеды Converse x Carhartt Chuck 70 OX</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16.300.₽</t>
+          <t>11.500.₽</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fdc/296_296_2/fdcab0e4271fc593d0dc2dbca4b630b4.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ab7/296_296_2/ab7f1ee7373c8e2c66a440ba55b381df.jpg </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-carchartt-chuck-70-ox-171238/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 OX x GOLF WANG</t>
+          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13.200.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e08/296_296_2/e08a58dd412f316675832c861c941994.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e33/296_296_2/e3336c4ddb34df6115445293375c8b1e.jpg </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-173189/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Кеды Converse x Carhartt Chuck 70 OX</t>
+          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11.500.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ab7/296_296_2/ab7f1ee7373c8e2c66a440ba55b381df.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/393/296_296_2/3934245cb0388e231c32f8a705ab8967.jpg </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-173190/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
+          <t>Кеды Converse  x Carhartt WIP Chuck 70 Hi Covert</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>12.490.₽</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e33/296_296_2/e3336c4ddb34df6115445293375c8b1e.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8ed/296_296_2/8edce77676cea0ffc0c9b12d4e09d5ac.jpg </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-covert-x-carhartt-wip-169221-5750/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
+          <t>Кеды Converse Chuck 70 x Golf Wang</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>9.400.₽</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/393/296_296_2/3934245cb0388e231c32f8a705ab8967.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/911/296_296_2/9115ee367194c3e5923a2929f58b838a.JPG </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-golf-wang-chuck-70-170011/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Кеды Converse  x Carhartt WIP Chuck 70 Hi Covert</t>
+          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>12.490.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8ed/296_296_2/8edce77676cea0ffc0c9b12d4e09d5ac.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c69/296_296_2/c691863f33e49b9c0064a11e132d566f.jpg </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-winter-2-0-hi-172057/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 x Golf Wang</t>
+          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>9.400.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/911/296_296_2/9115ee367194c3e5923a2929f58b838a.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/829/296_296_2/829d4c68c14f273ebc3c9a0fe6db4708.jpg </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A00911/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
+          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1030,143 +1205,144 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c69/296_296_2/c691863f33e49b9c0064a11e132d566f.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50c/296_296_2/50c9ed96c30e4507a64e66d191163e29.jpg </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A00912/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
+          <t>Кеды Converse Fastbreak Pro Mid</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>13.500.₽</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/829/296_296_2/829d4c68c14f273ebc3c9a0fe6db4708.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/94f/296_296_2/94f5eb301c8f419b86d11f49dd21cc06.jpg </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/fastbreak-pro-mid-A01703/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
+          <t>Кеды Converse Pro Leather OX</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>14.300.₽</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50c/296_296_2/50c9ed96c30e4507a64e66d191163e29.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c81/296_296_2/c815c24644a319e1059be1b880207e25.jpg </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/pro-leather-ox-A01649/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Кеды Converse Fastbreak Pro Mid</t>
+          <t>Кеды Converse x Sean Pablo One Star Pro OX</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>13.500.₽</t>
+          <t>12.800.₽</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/94f/296_296_2/94f5eb301c8f419b86d11f49dd21cc06.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dd6/296_296_2/dd69c6f283db58b8c1d2777b8b3a5d25.jpg </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/x-sean-pablo-one-star-pro-ox-173215/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Кеды Converse Pro Leather OX</t>
+          <t>Кеды Converse Chuck 70 OX</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>14.300.₽</t>
+          <t>13.500.₽</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c81/296_296_2/c815c24644a319e1059be1b880207e25.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dae/296_296_2/dae060e5767d35728a80aa51eeb7ded8.jpg </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-162058/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Кеды Converse x Sean Pablo One Star Pro OX</t>
+          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>12.800.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dd6/296_296_2/dd69c6f283db58b8c1d2777b8b3a5d25.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b4/296_296_2/5b4176798670d4ff703ee9d7b85dac38.jpg </t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-winter-2-0-hi-171425/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 OX</t>
+          <t>Кеды Converse Chuck 70 Tape</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>13.500.₽</t>
+          <t>11.390.₽</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dae/296_296_2/dae060e5767d35728a80aa51eeb7ded8.jpg </t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>17.500.₽</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b4/296_296_2/5b4176798670d4ff703ee9d7b85dac38.jpg </t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Кеды Converse Chuck 70 Tape</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>11.390.₽</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
           <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8b6/296_296_2/8b68b5468810e0ac13a77133c2c45680.jpg </t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-tape-170904/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to check existing of table
</commit_message>
<xml_diff>
--- a/gumshoes.xlsx
+++ b/gumshoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,315 +469,315 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
+          <t>Кеды Converse x Naturally Digital Chuck 70 OX</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>13.500.₽</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7fa/296_296_2/7fadf0fd1bcb0f9635cab145ae4cec40.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/74a/296_296_2/0zprnekw2ewy5x9nobcnbxze9mlwzbr3.jpg </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A01330/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-A04335/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 OX</t>
+          <t>Кеды Converse Chuck 70 Plus Hi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>13.500.₽</t>
+          <t>16.000.₽</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/196/296_296_2/on8f5v0t97na2ses6mlqpfpkm7ba6is1.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b09/296_296_2/rro1ooz0q455eplhjugznzgzjti9cwbx.jpg </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-A02771/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-plus-hi-A02871/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Кеды Converse x Naturally Digital Chuck 70 OX</t>
+          <t>Кеды Converse Run Star Motion CX HI</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13.500.₽</t>
+          <t>18.900.₽</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/74a/296_296_2/0zprnekw2ewy5x9nobcnbxze9mlwzbr3.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f4e/296_296_2/56231v21p308mqunndoa6a6ay31tepzk.jpg </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-A04335/</t>
+          <t>https://sneakerhead.ru/shoes/keds/run-star-motion-cx-hi-A05110/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 Plus Hi</t>
+          <t>Кеды Converse Run Star Motion CX HI</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16.000.₽</t>
+          <t>19.900.₽</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b09/296_296_2/rro1ooz0q455eplhjugznzgzjti9cwbx.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/59a/296_296_2/btqj3q49w2a4vtsk5txu8u92mhki1qmo.jpg </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-plus-hi-A02871/</t>
+          <t>https://sneakerhead.ru/shoes/keds/run-star-motion-cx-hi-A04334/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Кеды Converse Run Star Motion CX HI</t>
+          <t>Кеды Converse One Star Pro OX</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18.900.₽</t>
+          <t>13.900.₽</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f4e/296_296_2/56231v21p308mqunndoa6a6ay31tepzk.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/755/296_296_2/h70a0dqk6og8ncmuc559scitlisy3bg4.jpg </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/run-star-motion-cx-hi-A05110/</t>
+          <t>https://sneakerhead.ru/shoes/keds/one-star-pro-ox-A04242/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Кеды Converse Run Star Motion CX HI</t>
+          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>19.900.₽</t>
+          <t>17.900.₽</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/59a/296_296_2/btqj3q49w2a4vtsk5txu8u92mhki1qmo.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/924/296_296_2/9247324f208d8ea6585ef112726fd8cf.jpg </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/run-star-motion-cx-hi-A04334/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A01765/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Кеды Converse One Star Pro OX</t>
+          <t>Кеды Converse Run Star Hike Hi</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13.900.₽</t>
+          <t>17.800.₽</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/755/296_296_2/h70a0dqk6og8ncmuc559scitlisy3bg4.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7a1/296_296_2/7a1944071666efd11a4c0aed92011ab6.jpg </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/one-star-pro-ox-A04242/</t>
+          <t>https://sneakerhead.ru/shoes/keds/run-star-hike-hi-A01650/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 AT-CX Hi</t>
+          <t>Кеды Converse Weapon CX Mid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15.500.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aa7/296_296_2/aq3ojiv2ydjahpzlf1qvbfvbtcxqldhq.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e6c/296_296_2/e6c0637cb708f993f9afba97bf03a7bb.jpg </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-at-cx-hi-A02776/</t>
+          <t>https://sneakerhead.ru/shoes/keds/weapon-cx-mid-A03230/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
+          <t>Кеды Converse x CLOT Jack Purcell OX</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17.900.₽</t>
+          <t>16.000.₽</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/924/296_296_2/9247324f208d8ea6585ef112726fd8cf.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e10/296_296_2/e102471599195bdf15459dfb523ba3bb.jpg </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A01765/</t>
+          <t>https://sneakerhead.ru/shoes/keds/jack-purcell-ox-A00322/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Кеды Converse Run Star Hike Hi</t>
+          <t>Кеды Converse x CLOT Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17.800.₽</t>
+          <t>17.200.₽</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7a1/296_296_2/7a1944071666efd11a4c0aed92011ab6.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9ec/296_296_2/9ec888598a86778150bc01c8b4ce948e.jpg </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/run-star-hike-hi-A01650/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A00321/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Кеды Converse Weapon CX Mid</t>
+          <t>Кеды Converse x Come Tees Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>17.100.₽</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e6c/296_296_2/e6c0637cb708f993f9afba97bf03a7bb.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/05d/296_296_2/05dc34874b3fc00765a1ace5f2c703ae.jpg </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/weapon-cx-mid-A03230/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A01762/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Кеды Converse x CLOT Jack Purcell OX</t>
+          <t>Кеды Converse Chuck 70 Plus Hi</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16.000.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e10/296_296_2/e102471599195bdf15459dfb523ba3bb.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a0c/296_296_2/a0c79f03ba520eb75a4ea630fc6d6d07.jpg </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/jack-purcell-ox-A00322/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-plus-hi-A00866/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Кеды Converse x CLOT Chuck 70 Hi</t>
+          <t>Кеды Vans Classic Slip-On 98 DX</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17.200.₽</t>
+          <t>7.290.₽</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9ec/296_296_2/9ec888598a86778150bc01c8b4ce948e.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/25a/296_296_2/25a095a37f2927fe49772808bb99aee4.jpg </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A00321/</t>
+          <t>https://sneakerhead.ru/shoes/keds/classic-slip-on-99-DX-VA3JEXPU1/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Кеды Converse x Come Tees Chuck 70 Hi</t>
+          <t>Кеды Converse x Carhartt Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17.100.₽</t>
+          <t>11.900.₽</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/05d/296_296_2/05dc34874b3fc00765a1ace5f2c703ae.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/21c/296_296_2/21cc62f5696f9784250ae1f2ffbcc324.jpg </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A01762/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-carhartt-chuck-70-hi-171237/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 Plus Hi</t>
+          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -787,437 +787,437 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a0c/296_296_2/a0c79f03ba520eb75a4ea630fc6d6d07.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aef/296_296_2/aefc82a9c733ffc85cdfec5a013841f5.jpg </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-plus-hi-A00866/</t>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A01329/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Кеды Vans Classic Slip-On 98 DX</t>
+          <t xml:space="preserve">Кеды Converse x Peanuts One Star OX </t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7.290.₽</t>
+          <t>16.300.₽</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/25a/296_296_2/25a095a37f2927fe49772808bb99aee4.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/558/296_296_2/558930bbdafb92eb1477086be36a9f25.jpg </t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/classic-slip-on-99-DX-VA3JEXPU1/</t>
+          <t>https://sneakerhead.ru/shoes/keds/one-star-ox-x-peanuts-A01873/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Кеды Converse x Carhartt Chuck 70 Hi</t>
+          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11.900.₽</t>
+          <t>15.300.₽</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/21c/296_296_2/21cc62f5696f9784250ae1f2ffbcc324.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/990/296_296_2/990d5a6329394486464fcd7680e09da6.jpg </t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-carhartt-chuck-70-hi-171237/</t>
+          <t>https://sneakerhead.ru/shoes/keds/skid-grip-ox-x-john-elliott-172577/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
+          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>15.300.₽</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aef/296_296_2/aefc82a9c733ffc85cdfec5a013841f5.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f8/296_296_2/7f89ac7135e6d3c969fdcca189ae6ab8.jpg </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A01329/</t>
+          <t>https://sneakerhead.ru/shoes/keds/skid-grip-ox-x-john-elliott-172578/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Кеды Converse x Golf Le Fleur GLF 2.0 OX</t>
+          <t>Кеды Converse x Joshua Vides Weapon CX Hi</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14.500.₽</t>
+          <t>19.300.₽</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dee/296_296_2/dee01e54df7f8ac297ab6bd21d052bcf.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bd3/296_296_2/bd3ba0a707a4fe8002fa94c1e2742d99.jpg </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-golf-le-fleur-glf-2-0-ox-173186/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-joshua-vides-weapon-cx-hi-A00715/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кеды Converse x Peanuts One Star OX </t>
+          <t>Кеды Converse x Carhartt Fastbreak Pro Mid</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16.300.₽</t>
+          <t>11.100.₽</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/558/296_296_2/558930bbdafb92eb1477086be36a9f25.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8de/296_296_2/8de985a56482f5b6c49dd439297fba5c.jpg </t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/one-star-ox-x-peanuts-A01873/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-carhartt-fastbreak-pro-mid-172583/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
+          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>15.300.₽</t>
+          <t>16.300.₽</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/990/296_296_2/990d5a6329394486464fcd7680e09da6.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fdc/296_296_2/fdcab0e4271fc593d0dc2dbca4b630b4.jpg </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/skid-grip-ox-x-john-elliott-172577/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A02052/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кеды Converse x John Elliott Skid Grip OX </t>
+          <t>Кеды Converse Chuck 70 OX x GOLF WANG</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>15.300.₽</t>
+          <t>13.200.₽</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f8/296_296_2/7f89ac7135e6d3c969fdcca189ae6ab8.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e08/296_296_2/e08a58dd412f316675832c861c941994.jpg </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/skid-grip-ox-x-john-elliott-172578/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-wang-A01798/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Кеды Converse x Joshua Vides Weapon CX Hi</t>
+          <t>Кеды Converse x Carhartt Chuck 70 OX</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>19.300.₽</t>
+          <t>11.500.₽</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bd3/296_296_2/bd3ba0a707a4fe8002fa94c1e2742d99.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ab7/296_296_2/ab7f1ee7373c8e2c66a440ba55b381df.jpg </t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-joshua-vides-weapon-cx-hi-A00715/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-carchartt-chuck-70-ox-171238/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Кеды Converse x Carhartt Fastbreak Pro Mid</t>
+          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11.100.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8de/296_296_2/8de985a56482f5b6c49dd439297fba5c.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e33/296_296_2/e3336c4ddb34df6115445293375c8b1e.jpg </t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-carhartt-fastbreak-pro-mid-172583/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-173189/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
+          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16.300.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fdc/296_296_2/fdcab0e4271fc593d0dc2dbca4b630b4.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/393/296_296_2/3934245cb0388e231c32f8a705ab8967.jpg </t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A02052/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-173190/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 OX x GOLF WANG</t>
+          <t>Кеды Converse  x Carhartt WIP Chuck 70 Hi Covert</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13.200.₽</t>
+          <t>12.490.₽</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e08/296_296_2/e08a58dd412f316675832c861c941994.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8ed/296_296_2/8edce77676cea0ffc0c9b12d4e09d5ac.jpg </t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-wang-A01798/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-covert-x-carhartt-wip-169221-5750/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Кеды Converse x Carhartt Chuck 70 OX</t>
+          <t>Кеды Converse Chuck 70 x Golf Wang</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11.500.₽</t>
+          <t>9.400.₽</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ab7/296_296_2/ab7f1ee7373c8e2c66a440ba55b381df.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/911/296_296_2/9115ee367194c3e5923a2929f58b838a.JPG </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-carchartt-chuck-70-ox-171238/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-golf-wang-chuck-70-170011/</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
+          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e33/296_296_2/e3336c4ddb34df6115445293375c8b1e.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c69/296_296_2/c691863f33e49b9c0064a11e132d566f.jpg </t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-173189/</t>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-winter-2-0-hi-172057/</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Кеды Converse x Golf Wang Chuck 70 OX</t>
+          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/393/296_296_2/3934245cb0388e231c32f8a705ab8967.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/829/296_296_2/829d4c68c14f273ebc3c9a0fe6db4708.jpg </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-x-golf-173190/</t>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A00911/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Кеды Converse  x Carhartt WIP Chuck 70 Hi Covert</t>
+          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>12.490.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8ed/296_296_2/8edce77676cea0ffc0c9b12d4e09d5ac.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50c/296_296_2/50c9ed96c30e4507a64e66d191163e29.jpg </t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-covert-x-carhartt-wip-169221-5750/</t>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A00912/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 x Golf Wang</t>
+          <t>Кеды Converse Fastbreak Pro Mid</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>9.400.₽</t>
+          <t>13.500.₽</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/911/296_296_2/9115ee367194c3e5923a2929f58b838a.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/94f/296_296_2/94f5eb301c8f419b86d11f49dd21cc06.jpg </t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-golf-wang-chuck-70-170011/</t>
+          <t>https://sneakerhead.ru/shoes/keds/fastbreak-pro-mid-A01703/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
+          <t>Кеды Converse Pro Leather OX</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>14.300.₽</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c69/296_296_2/c691863f33e49b9c0064a11e132d566f.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c81/296_296_2/c815c24644a319e1059be1b880207e25.jpg </t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-winter-2-0-hi-172057/</t>
+          <t>https://sneakerhead.ru/shoes/keds/pro-leather-ox-A01649/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
+          <t>Кеды Converse x Sean Pablo One Star Pro OX</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>12.800.₽</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/829/296_296_2/829d4c68c14f273ebc3c9a0fe6db4708.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dd6/296_296_2/dd69c6f283db58b8c1d2777b8b3a5d25.jpg </t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A00911/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-sean-pablo-one-star-pro-ox-173215/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Кеды Converse CTAS Lugged 2.0 CC Hi</t>
+          <t>Кеды Converse Chuck 70 Mid Sea S x Undftd</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>12.080.₽</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50c/296_296_2/50c9ed96c30e4507a64e66d191163e29.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/91c/296_296_2/91c4a8b2a6593af196f5acff854cbf5d.jpg </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-2-0-cc-hi-A00912/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-mid-sea-s-x-undftd-172397/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Кеды Converse Fastbreak Pro Mid</t>
+          <t>Кеды Converse Chuck 70 OX</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1227,120 +1227,54 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/94f/296_296_2/94f5eb301c8f419b86d11f49dd21cc06.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dae/296_296_2/dae060e5767d35728a80aa51eeb7ded8.jpg </t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/fastbreak-pro-mid-A01703/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-162058/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Кеды Converse Pro Leather OX</t>
+          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>14.300.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c81/296_296_2/c815c24644a319e1059be1b880207e25.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b4/296_296_2/5b4176798670d4ff703ee9d7b85dac38.jpg </t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/pro-leather-ox-A01649/</t>
+          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-winter-2-0-hi-171425/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Кеды Converse x Sean Pablo One Star Pro OX</t>
+          <t>Кеды Converse Chuck 70 Tape</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>12.800.₽</t>
+          <t>11.390.₽</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dd6/296_296_2/dd69c6f283db58b8c1d2777b8b3a5d25.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8b6/296_296_2/8b68b5468810e0ac13a77133c2c45680.jpg </t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
-        <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-sean-pablo-one-star-pro-ox-173215/</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Кеды Converse Chuck 70 OX</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>13.500.₽</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/dae/296_296_2/dae060e5767d35728a80aa51eeb7ded8.jpg </t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-ox-162058/</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Кеды Converse CTAS Lugged Winter 2.0 Hi</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>17.500.₽</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b4/296_296_2/5b4176798670d4ff703ee9d7b85dac38.jpg </t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>https://sneakerhead.ru/shoes/keds/ctas-lugged-winter-2-0-hi-171425/</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Кеды Converse Chuck 70 Tape</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>11.390.₽</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8b6/296_296_2/8b68b5468810e0ac13a77133c2c45680.jpg </t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
         <is>
           <t>https://sneakerhead.ru/shoes/keds/chuck-70-tape-170904/</t>
         </is>

</xml_diff>

<commit_message>
checking existing of table, fixed "added shoes" list and viewing of the first card, refactored names
</commit_message>
<xml_diff>
--- a/gumshoes.xlsx
+++ b/gumshoes.xlsx
@@ -579,154 +579,154 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
+          <t>Кеды Converse Chuck 70 AT-CX Hi</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17.900.₽</t>
+          <t>15.500.₽</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/924/296_296_2/9247324f208d8ea6585ef112726fd8cf.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/aa7/296_296_2/aq3ojiv2ydjahpzlf1qvbfvbtcxqldhq.jpg </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A01765/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-at-cx-hi-A02776/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Кеды Converse Run Star Hike Hi</t>
+          <t>Кеды Converse x Stussy Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17.800.₽</t>
+          <t>17.900.₽</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7a1/296_296_2/7a1944071666efd11a4c0aed92011ab6.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/924/296_296_2/9247324f208d8ea6585ef112726fd8cf.jpg </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/run-star-hike-hi-A01650/</t>
+          <t>https://sneakerhead.ru/shoes/keds/x-stussy-chuck-70-hi-A01765/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Кеды Converse Weapon CX Mid</t>
+          <t>Кеды Converse Run Star Hike Hi</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>17.800.₽</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e6c/296_296_2/e6c0637cb708f993f9afba97bf03a7bb.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7a1/296_296_2/7a1944071666efd11a4c0aed92011ab6.jpg </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/weapon-cx-mid-A03230/</t>
+          <t>https://sneakerhead.ru/shoes/keds/run-star-hike-hi-A01650/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Кеды Converse x CLOT Jack Purcell OX</t>
+          <t>Кеды Converse Weapon CX Mid</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16.000.₽</t>
+          <t>17.500.₽</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e10/296_296_2/e102471599195bdf15459dfb523ba3bb.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e6c/296_296_2/e6c0637cb708f993f9afba97bf03a7bb.jpg </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/jack-purcell-ox-A00322/</t>
+          <t>https://sneakerhead.ru/shoes/keds/weapon-cx-mid-A03230/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Кеды Converse x CLOT Chuck 70 Hi</t>
+          <t>Кеды Converse x CLOT Jack Purcell OX</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17.200.₽</t>
+          <t>16.000.₽</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9ec/296_296_2/9ec888598a86778150bc01c8b4ce948e.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e10/296_296_2/e102471599195bdf15459dfb523ba3bb.jpg </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A00321/</t>
+          <t>https://sneakerhead.ru/shoes/keds/jack-purcell-ox-A00322/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Кеды Converse x Come Tees Chuck 70 Hi</t>
+          <t>Кеды Converse x CLOT Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17.100.₽</t>
+          <t>17.200.₽</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/05d/296_296_2/05dc34874b3fc00765a1ace5f2c703ae.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9ec/296_296_2/9ec888598a86778150bc01c8b4ce948e.jpg </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A01762/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A00321/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Кеды Converse Chuck 70 Plus Hi</t>
+          <t>Кеды Converse x Come Tees Chuck 70 Hi</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17.500.₽</t>
+          <t>17.100.₽</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a0c/296_296_2/a0c79f03ba520eb75a4ea630fc6d6d07.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/05d/296_296_2/05dc34874b3fc00765a1ace5f2c703ae.jpg </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru/shoes/keds/chuck-70-plus-hi-A00866/</t>
+          <t>https://sneakerhead.ru/shoes/keds/chuck-70-hi-A01762/</t>
         </is>
       </c>
     </row>

</xml_diff>